<commit_message>
Updated excel reading logic
</commit_message>
<xml_diff>
--- a/src/assets/Destination.xlsx
+++ b/src/assets/Destination.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Siva\Personal\GitHub\Angular\angular-excel\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F144D6D5-B9A3-486F-9C1B-A8E529BAA8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69803904-5A43-49FE-982B-36DCEB75A6F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Siva</t>
   </si>
@@ -33,7 +34,16 @@
     <t>Sankar</t>
   </si>
   <si>
-    <t>Ram</t>
+    <t>Ra</t>
+  </si>
+  <si>
+    <t>fgf</t>
+  </si>
+  <si>
+    <t>fdgfd</t>
+  </si>
+  <si>
+    <t>fdg</t>
   </si>
 </sst>
 </file>
@@ -353,8 +363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -366,12 +376,45 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3B567A8-3ECA-4F7E-8B06-7CB73E081285}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>